<commit_message>
Various additions and footer added
</commit_message>
<xml_diff>
--- a/src/assets/cnic_sample.xlsx
+++ b/src/assets/cnic_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniyaalbeg/Documents/cs/MERN/corona_ration/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniyaalbeg/Documents/cs/MERN/mc/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C9B7EA-A1CF-624A-8ACA-1D9C4A891CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7DE0AD-4AE8-4942-B478-1695B7D789CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{DDB41715-FD77-BA48-877B-511F3350BABE}"/>
   </bookViews>
@@ -50,21 +50,29 @@
     <t>address</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>other info</t>
-  </si>
-  <si>
-    <t>contactNumber</t>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Other Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,21 +96,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -113,6 +206,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6A806BB-74DA-964A-B6A5-3A3EC54C6CF7}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11">
+  <autoFilter ref="A1:H1048576" xr:uid="{AAE98CB3-6E60-CE4F-8DDC-5CAA15421B38}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8CFB73E9-ECF0-3748-A14B-C25761ABC270}" name="CNIC " dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{5AF80102-36F3-3040-9742-5100D4CCCAC7}" name="Name" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{18CE2D28-108C-6C44-A5E3-138054C96525}" name="Contact Number" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{BD14363C-19F3-0247-83C9-BE72BB6369E2}" name="address" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{51C4A098-30C0-3F4F-8428-55629F41A60C}" name="DOB" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{98EC560F-3B01-134E-8A83-C6406145CEEC}" name="Family Size" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F6C54037-1B86-A449-BDBF-A4F96D69E8BD}" name="Gender" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{83C29CF6-CEF6-EC46-B011-A21B023B89C5}" name="Other Info" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,7 +525,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,37 +535,42 @@
     <col min="4" max="4" width="25.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wpjNZL8OXLoJx75KHbh5PWcxWx0wkOhkn33vfks6ETBv5AsC3lHlLAFrR4goKp+9hzleROxvaUJWS0tTXN0aBw==" saltValue="wMDCjTQp9g8q7ZGd7y1mFw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="GNrL23IJTuCY34JDcuYuGVgaxwYqTe5vQJsQbPJeJbgmupy0v95U82EugiEgYpg7xuMpWakID948XfDxPQ70PQ==" saltValue="3aXqNBDlbYWPjfJJarYwaw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>